<commit_message>
解决Zonal Statistics as Table出错问题
</commit_message>
<xml_diff>
--- a/data/公报图表模板.xlsx
+++ b/data/公报图表模板.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2430" windowHeight="1140" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2430" windowHeight="1140"/>
   </bookViews>
   <sheets>
     <sheet name="分区统计" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
   <si>
     <t>总</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -121,78 +121,6 @@
   </si>
   <si>
     <t>地闪总数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>宁波</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>湖州</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>嘉兴</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>绍兴</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>金华</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>台州</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>温州</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>衢州</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>丽水</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>舟山</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>总计</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>越城区</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>柯桥区</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>上虞区</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>诸暨市</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>嵊州市</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>新昌县</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>杭州</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -599,8 +527,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="198183456"/>
-        <c:axId val="198184016"/>
+        <c:axId val="187629024"/>
+        <c:axId val="187629584"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -887,11 +815,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="198185136"/>
-        <c:axId val="198184576"/>
+        <c:axId val="187630704"/>
+        <c:axId val="187630144"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="198183456"/>
+        <c:axId val="187629024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -997,7 +925,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="198184016"/>
+        <c:crossAx val="187629584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1005,7 +933,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="198184016"/>
+        <c:axId val="187629584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1051,7 +979,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1114,12 +1041,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="198183456"/>
+        <c:crossAx val="187629024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="198184576"/>
+        <c:axId val="187630144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1160,7 +1087,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1225,12 +1151,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="198185136"/>
+        <c:crossAx val="187630704"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="198185136"/>
+        <c:axId val="187630704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1239,7 +1165,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="198184576"/>
+        <c:crossAx val="187630144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1256,7 +1182,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1624,8 +1549,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="198189056"/>
-        <c:axId val="198189616"/>
+        <c:axId val="187634624"/>
+        <c:axId val="187635184"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1936,11 +1861,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="198190736"/>
-        <c:axId val="198190176"/>
+        <c:axId val="187636304"/>
+        <c:axId val="187635744"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="198189056"/>
+        <c:axId val="187634624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2045,7 +1970,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="198189616"/>
+        <c:crossAx val="187635184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2053,7 +1978,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="198189616"/>
+        <c:axId val="187635184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2122,7 +2047,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2185,12 +2109,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="198189056"/>
+        <c:crossAx val="187634624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="198190176"/>
+        <c:axId val="187635744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2230,7 +2154,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2293,12 +2216,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="198190736"/>
+        <c:crossAx val="187636304"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="198190736"/>
+        <c:axId val="187636304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2307,7 +2230,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="198190176"/>
+        <c:crossAx val="187635744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2324,7 +2247,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2648,8 +2570,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="198193536"/>
-        <c:axId val="198194096"/>
+        <c:axId val="187639104"/>
+        <c:axId val="187639664"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2775,11 +2697,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="198195216"/>
-        <c:axId val="198194656"/>
+        <c:axId val="189075056"/>
+        <c:axId val="187640224"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="198193536"/>
+        <c:axId val="187639104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2886,7 +2808,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="198194096"/>
+        <c:crossAx val="187639664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2894,7 +2816,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="198194096"/>
+        <c:axId val="187639664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3024,12 +2946,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="198193536"/>
+        <c:crossAx val="187639104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="198194656"/>
+        <c:axId val="187640224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3123,12 +3045,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="198195216"/>
+        <c:crossAx val="189075056"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="198195216"/>
+        <c:axId val="189075056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3137,7 +3059,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="198194656"/>
+        <c:crossAx val="187640224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3478,8 +3400,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="198198016"/>
-        <c:axId val="198198576"/>
+        <c:axId val="189077856"/>
+        <c:axId val="189078416"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -3605,11 +3527,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="199130832"/>
-        <c:axId val="198199136"/>
+        <c:axId val="189079536"/>
+        <c:axId val="189078976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="198198016"/>
+        <c:axId val="189077856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3716,7 +3638,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="198198576"/>
+        <c:crossAx val="189078416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3724,7 +3646,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="198198576"/>
+        <c:axId val="189078416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3854,12 +3776,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="198198016"/>
+        <c:crossAx val="189077856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="198199136"/>
+        <c:axId val="189078976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3953,12 +3875,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="199130832"/>
+        <c:crossAx val="189079536"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="199130832"/>
+        <c:axId val="189079536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3967,7 +3889,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="198199136"/>
+        <c:crossAx val="189078976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6730,8 +6652,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -6746,124 +6668,52 @@
       <c r="A1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="J1" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="K1" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="L1" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="M1" s="14" t="s">
-        <v>37</v>
-      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A2" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="13">
-        <v>15616</v>
-      </c>
-      <c r="C2" s="13">
-        <v>19374</v>
-      </c>
-      <c r="D2" s="13">
-        <v>3011</v>
-      </c>
-      <c r="E2" s="13">
-        <v>4161</v>
-      </c>
-      <c r="F2" s="13">
-        <v>9272</v>
-      </c>
-      <c r="G2" s="13">
-        <v>19839</v>
-      </c>
-      <c r="H2" s="13">
-        <v>25476</v>
-      </c>
-      <c r="I2" s="13">
-        <v>12942</v>
-      </c>
-      <c r="J2" s="13">
-        <v>17398</v>
-      </c>
-      <c r="K2" s="13">
-        <v>16926</v>
-      </c>
-      <c r="L2" s="13">
-        <v>1598</v>
-      </c>
-      <c r="M2" s="13">
-        <v>145613</v>
-      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A3" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="12">
-        <v>0.93</v>
-      </c>
-      <c r="C3" s="12">
-        <v>1.46</v>
-      </c>
-      <c r="D3" s="12">
-        <v>0.52</v>
-      </c>
-      <c r="E3" s="12">
-        <v>0.71</v>
-      </c>
-      <c r="F3" s="12">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="G3" s="12">
-        <v>1.82</v>
-      </c>
-      <c r="H3" s="12">
-        <v>1.97</v>
-      </c>
-      <c r="I3" s="12">
-        <v>0.82</v>
-      </c>
-      <c r="J3" s="12">
-        <v>1.97</v>
-      </c>
-      <c r="K3" s="12">
-        <v>0.98</v>
-      </c>
-      <c r="L3" s="12">
-        <v>0.12</v>
-      </c>
-      <c r="M3" s="12">
-        <v>1.1299999999999999</v>
-      </c>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.15">
       <c r="B4" s="12"/>
@@ -6883,27 +6733,13 @@
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="G5" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="H5" s="15" t="s">
-        <v>37</v>
-      </c>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
       <c r="I5" s="15"/>
       <c r="J5" s="15"/>
       <c r="K5" s="15"/>
@@ -6914,27 +6750,13 @@
       <c r="A6" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="12">
-        <v>106</v>
-      </c>
-      <c r="C6" s="12">
-        <v>487</v>
-      </c>
-      <c r="D6" s="12">
-        <v>561</v>
-      </c>
-      <c r="E6" s="12">
-        <v>4788</v>
-      </c>
-      <c r="F6" s="12">
-        <v>1970</v>
-      </c>
-      <c r="G6" s="12">
-        <v>1360</v>
-      </c>
-      <c r="H6" s="12">
-        <v>9272</v>
-      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
       <c r="K6" s="12"/>
@@ -6945,27 +6767,13 @@
       <c r="A7" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="12">
-        <v>0.22</v>
-      </c>
-      <c r="C7" s="12">
-        <v>0.46</v>
-      </c>
-      <c r="D7" s="12">
-        <v>0.4</v>
-      </c>
-      <c r="E7" s="12">
-        <v>2.0699999999999998</v>
-      </c>
-      <c r="F7" s="12">
-        <v>1.1100000000000001</v>
-      </c>
-      <c r="G7" s="12">
-        <v>1.1100000000000001</v>
-      </c>
-      <c r="H7" s="12">
-        <v>1.1200000000000001</v>
-      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
       <c r="I7" s="12"/>
       <c r="J7" s="12"/>
       <c r="K7" s="12"/>
@@ -6976,27 +6784,13 @@
       <c r="A8" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="12">
-        <v>0.59</v>
-      </c>
-      <c r="C8" s="12">
-        <v>2.44</v>
-      </c>
-      <c r="D8" s="12">
-        <v>0.84</v>
-      </c>
-      <c r="E8" s="12">
-        <v>5.64</v>
-      </c>
-      <c r="F8" s="12">
-        <v>5.18</v>
-      </c>
-      <c r="G8" s="12">
-        <v>4.42</v>
-      </c>
-      <c r="H8" s="12">
-        <v>5.64</v>
-      </c>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
       <c r="I8" s="12"/>
       <c r="J8" s="12"/>
       <c r="K8" s="12"/>
@@ -7007,27 +6801,13 @@
       <c r="A9" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="12">
-        <v>0.11</v>
-      </c>
-      <c r="C9" s="12">
-        <v>0.11</v>
-      </c>
-      <c r="D9" s="12">
-        <v>0.11</v>
-      </c>
-      <c r="E9" s="12">
-        <v>0.26</v>
-      </c>
-      <c r="F9" s="12">
-        <v>0.2</v>
-      </c>
-      <c r="G9" s="12">
-        <v>0.47</v>
-      </c>
-      <c r="H9" s="12">
-        <v>0.11</v>
-      </c>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
       <c r="I9" s="12"/>
       <c r="J9" s="12"/>
       <c r="K9" s="12"/>
@@ -7038,27 +6818,13 @@
       <c r="A10" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="12">
-        <v>36</v>
-      </c>
-      <c r="C10" s="12">
-        <v>42</v>
-      </c>
-      <c r="D10" s="12">
-        <v>35</v>
-      </c>
-      <c r="E10" s="12">
-        <v>57</v>
-      </c>
-      <c r="F10" s="12">
-        <v>44</v>
-      </c>
-      <c r="G10" s="12">
-        <v>45</v>
-      </c>
-      <c r="H10" s="12">
-        <v>43</v>
-      </c>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
       <c r="I10" s="12"/>
       <c r="J10" s="12"/>
       <c r="K10" s="12"/>
@@ -7069,27 +6835,13 @@
       <c r="A11" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="12">
-        <v>43</v>
-      </c>
-      <c r="C11" s="12">
-        <v>52</v>
-      </c>
-      <c r="D11" s="12">
-        <v>41</v>
-      </c>
-      <c r="E11" s="12">
-        <v>67</v>
-      </c>
-      <c r="F11" s="12">
-        <v>54</v>
-      </c>
-      <c r="G11" s="12">
-        <v>66</v>
-      </c>
-      <c r="H11" s="12">
-        <v>67</v>
-      </c>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
       <c r="I11" s="12"/>
       <c r="J11" s="12"/>
       <c r="K11" s="12"/>
@@ -7100,27 +6852,13 @@
       <c r="A12" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="12">
-        <v>30</v>
-      </c>
-      <c r="C12" s="12">
-        <v>31</v>
-      </c>
-      <c r="D12" s="12">
-        <v>30</v>
-      </c>
-      <c r="E12" s="12">
-        <v>45</v>
-      </c>
-      <c r="F12" s="12">
-        <v>36</v>
-      </c>
-      <c r="G12" s="12">
-        <v>39</v>
-      </c>
-      <c r="H12" s="12">
-        <v>30</v>
-      </c>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
       <c r="I12" s="12"/>
       <c r="J12" s="12"/>
       <c r="K12" s="12"/>
@@ -8043,7 +7781,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>

</xml_diff>